<commit_message>
GEP_SpaceDust: six DustBunnies resources
</commit_message>
<xml_diff>
--- a/GEP_SpaceDust.xlsx
+++ b/GEP_SpaceDust.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Documents\GitHub\Grannus-Expansion-Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0801FD36-15B6-4353-AB67-A5A58D3E7F20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D0A3CE-539A-47FC-8D23-A5194F9C28D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21060" windowHeight="19155" xr2:uid="{CCF496B2-B669-4137-9B43-48A069A2A925}"/>
+    <workbookView xWindow="2085" yWindow="825" windowWidth="18675" windowHeight="19155" activeTab="3" xr2:uid="{CCF496B2-B669-4137-9B43-48A069A2A925}"/>
   </bookViews>
   <sheets>
     <sheet name="GEP_SpaceDust" sheetId="2" r:id="rId1"/>
     <sheet name="Details" sheetId="3" r:id="rId2"/>
     <sheet name="Atmo" sheetId="4" r:id="rId3"/>
+    <sheet name="Ring" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Atmo!$A$2:$T$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Atmo!$A$2:$U$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Details!$A$1:$I$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GEP_SpaceDust!$A$2:$T$24</definedName>
   </definedNames>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="141">
   <si>
     <t>Total</t>
   </si>
@@ -407,6 +408,54 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>g/cm^2</t>
+  </si>
+  <si>
+    <t>t/m^2</t>
+  </si>
+  <si>
+    <t>Surface density</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>Water Abundance</t>
+  </si>
+  <si>
+    <t>Rock Abundance</t>
+  </si>
+  <si>
+    <t>Saturn's rings</t>
+  </si>
+  <si>
+    <t>Outer radius</t>
+  </si>
+  <si>
+    <t>Inner radius</t>
+  </si>
+  <si>
+    <t>milliradii</t>
+  </si>
+  <si>
+    <t>Planet radius</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -497,7 +546,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -537,9 +586,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -572,14 +618,18 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -909,13 +959,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296BC83F-506F-402F-A907-28F8B7EE137D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,24 +983,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="E1" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
       <c r="S1" s="16"/>
     </row>
     <row r="2" spans="1:20" s="11" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
@@ -1014,7 +1065,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>12</v>
       </c>
@@ -1056,7 +1107,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="1">
-        <f>COUNTIFS(E3:R3,"&lt;&gt;",E3:R3,"&lt;&gt;-",E3:R3,"&lt;&gt;--")</f>
+        <f t="shared" ref="S3:S23" si="0">COUNTIFS(E3:R3,"&lt;&gt;",E3:R3,"&lt;&gt;-",E3:R3,"&lt;&gt;--")</f>
         <v>0</v>
       </c>
     </row>
@@ -1108,11 +1159,11 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="1">
-        <f>COUNTIFS(E4:R4,"&lt;&gt;",E4:R4,"&lt;&gt;-",E4:R4,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>12.1</v>
       </c>
@@ -1150,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="S5" s="1">
-        <f>COUNTIFS(E5:R5,"&lt;&gt;",E5:R5,"&lt;&gt;-",E5:R5,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1182,23 +1233,23 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="3" t="s">
-        <v>1</v>
+      <c r="N6" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="O6" s="3"/>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="8" t="s">
         <v>12</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3" t="s">
-        <v>12</v>
+      <c r="R6" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S6" s="1">
-        <f>COUNTIFS(E6:R6,"&lt;&gt;",E6:R6,"&lt;&gt;-",E6:R6,"&lt;&gt;--")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>12.2</v>
       </c>
@@ -1214,8 +1265,8 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="6" t="s">
-        <v>12</v>
+      <c r="H7" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -1228,8 +1279,8 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="1">
-        <f>COUNTIFS(E7:R7,"&lt;&gt;",E7:R7,"&lt;&gt;-",E7:R7,"&lt;&gt;--")</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1260,22 +1311,22 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="3" t="s">
+      <c r="N8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="S8" s="1">
-        <f>COUNTIFS(E8:R8,"&lt;&gt;",E8:R8,"&lt;&gt;-",E8:R8,"&lt;&gt;--")</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="T8" s="3"/>
     </row>
@@ -1311,19 +1362,19 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="3" t="s">
-        <v>1</v>
+      <c r="P9" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3" t="s">
-        <v>14</v>
+      <c r="R9" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S9" s="1">
-        <f>COUNTIFS(E9:R9,"&lt;&gt;",E9:R9,"&lt;&gt;-",E9:R9,"&lt;&gt;--")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
@@ -1361,11 +1412,11 @@
         <v>6</v>
       </c>
       <c r="S10" s="1">
-        <f>COUNTIFS(E10:R10,"&lt;&gt;",E10:R10,"&lt;&gt;-",E10:R10,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>12.4</v>
       </c>
@@ -1403,11 +1454,11 @@
         <v>6</v>
       </c>
       <c r="S11" s="1">
-        <f>COUNTIFS(E11:R11,"&lt;&gt;",E11:R11,"&lt;&gt;-",E11:R11,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>28</v>
       </c>
@@ -1445,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="S12" s="1">
-        <f>COUNTIFS(E12:R12,"&lt;&gt;",E12:R12,"&lt;&gt;-",E12:R12,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1478,23 +1529,23 @@
       <c r="L13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="M13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="3" t="s">
+      <c r="N13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="3" t="s">
-        <v>14</v>
+      <c r="R13" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S13" s="1">
-        <f>COUNTIFS(E13:R13,"&lt;&gt;",E13:R13,"&lt;&gt;-",E13:R13,"&lt;&gt;--")</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1530,16 +1581,18 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="3" t="s">
+      <c r="Q14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="R14" s="3"/>
+      <c r="R14" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="S14" s="1">
-        <f>COUNTIFS(E14:R14,"&lt;&gt;",E14:R14,"&lt;&gt;-",E14:R14,"&lt;&gt;--")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1577,7 +1630,7 @@
         <v>6</v>
       </c>
       <c r="S15" s="1">
-        <f>COUNTIFS(E15:R15,"&lt;&gt;",E15:R15,"&lt;&gt;-",E15:R15,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1606,26 +1659,26 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="M16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="P16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="1">
-        <f>COUNTIFS(E16:R16,"&lt;&gt;",E16:R16,"&lt;&gt;-",E16:R16,"&lt;&gt;--")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
@@ -1642,8 +1695,8 @@
       <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>12</v>
+      <c r="H17" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1656,21 +1709,21 @@
         <v>6</v>
       </c>
       <c r="O17" s="3"/>
-      <c r="P17" s="3" t="s">
-        <v>1</v>
+      <c r="P17" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>1</v>
+      <c r="R17" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S17" s="1">
-        <f>COUNTIFS(E17:R17,"&lt;&gt;",E17:R17,"&lt;&gt;-",E17:R17,"&lt;&gt;--")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
@@ -1708,7 +1761,7 @@
         <v>6</v>
       </c>
       <c r="S18" s="1">
-        <f>COUNTIFS(E18:R18,"&lt;&gt;",E18:R18,"&lt;&gt;-",E18:R18,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1737,26 +1790,26 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" s="3" t="s">
+      <c r="M19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="P19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="1">
-        <f>COUNTIFS(E19:R19,"&lt;&gt;",E19:R19,"&lt;&gt;-",E19:R19,"&lt;&gt;--")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>12.6</v>
       </c>
@@ -1772,8 +1825,8 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="6" t="s">
-        <v>12</v>
+      <c r="H20" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1782,23 +1835,23 @@
         <v>2</v>
       </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="3" t="s">
-        <v>1</v>
+      <c r="N20" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="O20" s="3"/>
-      <c r="P20" s="3" t="s">
-        <v>1</v>
+      <c r="P20" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="Q20" s="3"/>
-      <c r="R20" s="3" t="s">
-        <v>1</v>
+      <c r="R20" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S20" s="1">
-        <f>COUNTIFS(E20:R20,"&lt;&gt;",E20:R20,"&lt;&gt;-",E20:R20,"&lt;&gt;--")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1836,11 +1889,11 @@
         <v>6</v>
       </c>
       <c r="S21" s="1">
-        <f>COUNTIFS(E21:R21,"&lt;&gt;",E21:R21,"&lt;&gt;-",E21:R21,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
@@ -1878,11 +1931,11 @@
         <v>6</v>
       </c>
       <c r="S22" s="1">
-        <f>COUNTIFS(E22:R22,"&lt;&gt;",E22:R22,"&lt;&gt;-",E22:R22,"&lt;&gt;--")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>12.7</v>
       </c>
@@ -1906,20 +1959,20 @@
         <v>2</v>
       </c>
       <c r="M23" s="3"/>
-      <c r="N23" s="3" t="s">
-        <v>1</v>
+      <c r="N23" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="O23" s="3"/>
-      <c r="P23" s="3" t="s">
-        <v>1</v>
+      <c r="P23" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="Q23" s="3"/>
-      <c r="R23" s="3" t="s">
-        <v>1</v>
+      <c r="R23" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="S23" s="1">
-        <f>COUNTIFS(E23:R23,"&lt;&gt;",E23:R23,"&lt;&gt;-",E23:R23,"&lt;&gt;--")</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="U23"/>
     </row>
@@ -1928,68 +1981,77 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <f>COUNTIFS(E3:E23,"&lt;&gt;",E3:E23,"&lt;&gt;-",E3:E23,"&lt;&gt;--")</f>
+        <f t="shared" ref="E24:R24" si="1">COUNTIFS(E3:E23,"&lt;&gt;",E3:E23,"&lt;&gt;-",E3:E23,"&lt;&gt;--")</f>
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <f>COUNTIFS(F3:F23,"&lt;&gt;",F3:F23,"&lt;&gt;-",F3:F23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G24" s="1">
-        <f>COUNTIFS(G3:G23,"&lt;&gt;",G3:G23,"&lt;&gt;-",G3:G23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H24" s="1">
-        <f>COUNTIFS(H3:H23,"&lt;&gt;",H3:H23,"&lt;&gt;-",H3:H23,"&lt;&gt;--")</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="I24" s="1">
-        <f>COUNTIFS(I3:I23,"&lt;&gt;",I3:I23,"&lt;&gt;-",I3:I23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J24" s="1">
-        <f>COUNTIFS(J3:J23,"&lt;&gt;",J3:J23,"&lt;&gt;-",J3:J23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K24" s="1">
-        <f>COUNTIFS(K3:K23,"&lt;&gt;",K3:K23,"&lt;&gt;-",K3:K23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L24" s="1">
-        <f>COUNTIFS(L3:L23,"&lt;&gt;",L3:L23,"&lt;&gt;-",L3:L23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M24" s="1">
-        <f>COUNTIFS(M3:M23,"&lt;&gt;",M3:M23,"&lt;&gt;-",M3:M23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="N24" s="1">
-        <f>COUNTIFS(N3:N23,"&lt;&gt;",N3:N23,"&lt;&gt;-",N3:N23,"&lt;&gt;--")</f>
-        <v>7</v>
-      </c>
-      <c r="O24" s="1">
-        <f>COUNTIFS(O3:O23,"&lt;&gt;",O3:O23,"&lt;&gt;-",O3:O23,"&lt;&gt;--")</f>
+      <c r="P24" s="1">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="P24" s="1">
-        <f>COUNTIFS(P3:P23,"&lt;&gt;",P3:P23,"&lt;&gt;-",P3:P23,"&lt;&gt;--")</f>
-        <v>8</v>
-      </c>
       <c r="Q24" s="1">
-        <f>COUNTIFS(Q3:Q23,"&lt;&gt;",Q3:Q23,"&lt;&gt;-",Q3:Q23,"&lt;&gt;--")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R24" s="1">
-        <f>COUNTIFS(R3:R23,"&lt;&gt;",R3:R23,"&lt;&gt;-",R3:R23,"&lt;&gt;--")</f>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="T24" s="1" t="str">
         <f>"Ignored: "&amp;COUNTIF(E3:R23,"-")+COUNTIF(E3:R23,"--")</f>
-        <v>Ignored: 65</v>
+        <v>Ignored: 86</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T24" xr:uid="{4726FF84-1C5D-4B2E-92F2-FD7BAB7539E6}"/>
+  <autoFilter ref="A2:T24" xr:uid="{4726FF84-1C5D-4B2E-92F2-FD7BAB7539E6}">
+    <filterColumn colId="18">
+      <filters blank="1">
+        <filter val="2"/>
+        <filter val="4"/>
+        <filter val="5"/>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="E1:L1"/>
     <mergeCell ref="M1:R1"/>
@@ -2029,10 +2091,10 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H60" sqref="H60"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2399,7 @@
         <v>650000</v>
       </c>
       <c r="H10">
-        <f>ROUND(G10/600000*700000,-4)</f>
+        <f t="shared" ref="H10:H15" si="0">ROUND(G10/600000*700000,-4)</f>
         <v>760000</v>
       </c>
       <c r="I10" t="s">
@@ -2367,7 +2429,7 @@
         <v>550000</v>
       </c>
       <c r="H11">
-        <f>ROUND(G11/600000*700000,-4)</f>
+        <f t="shared" si="0"/>
         <v>640000</v>
       </c>
       <c r="I11" t="s">
@@ -2397,7 +2459,7 @@
         <v>600000</v>
       </c>
       <c r="H12">
-        <f>ROUND(G12/600000*700000,-4)</f>
+        <f t="shared" si="0"/>
         <v>700000</v>
       </c>
       <c r="I12" t="s">
@@ -2427,7 +2489,7 @@
         <v>2100000</v>
       </c>
       <c r="H13">
-        <f>ROUND(G13/600000*700000,-4)</f>
+        <f t="shared" si="0"/>
         <v>2450000</v>
       </c>
       <c r="I13" t="s">
@@ -2457,7 +2519,7 @@
         <v>1900000</v>
       </c>
       <c r="H14">
-        <f>ROUND(G14/600000*700000,-4)</f>
+        <f t="shared" si="0"/>
         <v>2220000</v>
       </c>
       <c r="I14" t="s">
@@ -2487,7 +2549,7 @@
         <v>2000000</v>
       </c>
       <c r="H15">
-        <f>ROUND(G15/600000*700000,-4)</f>
+        <f t="shared" si="0"/>
         <v>2330000</v>
       </c>
       <c r="I15" t="s">
@@ -3093,7 +3155,7 @@
       <c r="G36">
         <v>1.1E-5</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="17">
         <f>0.75*5.89773625228506E-06</f>
         <v>4.4233021892137952E-6</v>
       </c>
@@ -3123,7 +3185,7 @@
       <c r="G37">
         <v>1.2E-5</v>
       </c>
-      <c r="H37" s="18">
+      <c r="H37" s="17">
         <f>1.25*5.89773625228506E-06</f>
         <v>7.3721703153563242E-6</v>
       </c>
@@ -3182,7 +3244,7 @@
       <c r="G39">
         <v>3.8000000000000001E-7</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="17">
         <f>0.75*0.0000188587578898548</f>
         <v>1.4144068417391099E-5</v>
       </c>
@@ -3212,7 +3274,7 @@
       <c r="G40">
         <v>7.1999999999999999E-7</v>
       </c>
-      <c r="H40" s="18">
+      <c r="H40" s="17">
         <f>1.25*0.0000188587578898548</f>
         <v>2.3573447362318498E-5</v>
       </c>
@@ -3271,7 +3333,7 @@
       <c r="G42">
         <v>3.8000000000000001E-7</v>
       </c>
-      <c r="H42" s="18">
+      <c r="H42" s="17">
         <f>0.75*2.17677824899889E-07</f>
         <v>1.6325836867491676E-7</v>
       </c>
@@ -3301,7 +3363,7 @@
       <c r="G43">
         <v>7.1999999999999999E-7</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="17">
         <f>1.25*2.17677824899889E-07</f>
         <v>2.7209728112486122E-7</v>
       </c>
@@ -3360,7 +3422,7 @@
       <c r="G45">
         <v>3.8000000000000001E-7</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="17">
         <f>0.75*0.0000267625332984646</f>
         <v>2.0071899973848447E-5</v>
       </c>
@@ -3390,7 +3452,7 @@
       <c r="G46">
         <v>7.1999999999999999E-7</v>
       </c>
-      <c r="H46" s="18">
+      <c r="H46" s="17">
         <f>1.25*0.0000267625332984646</f>
         <v>3.345316662308075E-5</v>
       </c>
@@ -3449,7 +3511,7 @@
       <c r="G48">
         <v>3.8000000000000001E-7</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="17">
         <f>0.75*0.0000187151301468672</f>
         <v>1.40363476101504E-5</v>
       </c>
@@ -3479,7 +3541,7 @@
       <c r="G49">
         <v>7.1999999999999999E-7</v>
       </c>
-      <c r="H49" s="18">
+      <c r="H49" s="17">
         <f>1.25*0.0000187151301468672</f>
         <v>2.3393912683584001E-5</v>
       </c>
@@ -3525,38 +3587,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EBE8DB-83CB-4706-B275-37FEB6383766}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" style="19" customWidth="1"/>
-    <col min="20" max="20" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" style="18" customWidth="1"/>
+    <col min="21" max="22" width="12" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" style="17" customWidth="1"/>
+    <col min="25" max="25" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="33" t="s">
         <v>123</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -3565,97 +3635,121 @@
       <c r="E1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="P1" s="33" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="Q1" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="Q1" s="17" t="s">
+      <c r="R1" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-    </row>
-    <row r="2" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+    </row>
+    <row r="2" spans="1:26" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>116</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="M2" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="Q2" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="R2" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="S2" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="T2" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="U2" s="25" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V2" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="W2" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="X2" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y2" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z2" s="25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3">
         <v>59000</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>0.04</v>
       </c>
       <c r="D3">
@@ -3665,51 +3759,60 @@
       <c r="E3">
         <v>43.33</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <v>0.04</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="21">
         <v>0.95</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="21">
         <v>0.01</v>
       </c>
-      <c r="N3" s="37">
-        <f>S3/P3</f>
+      <c r="N3" s="35">
+        <f>T3/Q3</f>
         <v>1.2509278260489891E-6</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="36"/>
+      <c r="P3" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="20">
+      <c r="Q3" s="19">
         <f>101325/((8.31446261815324/E3*1000)*D3)/1000</f>
         <v>1.8858757889854774E-3</v>
       </c>
-      <c r="Q3">
-        <f>P3*G3</f>
+      <c r="R3">
+        <f>Q3*G3</f>
         <v>0</v>
       </c>
-      <c r="R3">
-        <f>P3*K3</f>
+      <c r="S3">
+        <f>Q3*K3</f>
         <v>0</v>
       </c>
-      <c r="S3" s="36">
-        <f>S$4</f>
+      <c r="T3" s="34">
+        <f>T$4</f>
         <v>2.3590945009140252E-9</v>
       </c>
-      <c r="T3" s="18">
-        <f>P3*J3</f>
+      <c r="U3" s="17">
+        <f>Q3*J3</f>
         <v>1.8858757889854775E-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W3" s="17">
+        <f>Q3*I3</f>
+        <v>1.7915819995362034E-3</v>
+      </c>
+      <c r="Z3" s="17">
+        <f>Q3*F3</f>
+        <v>7.5435031559419098E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
       <c r="B4">
         <v>72000</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>2</v>
       </c>
       <c r="D4">
@@ -3718,56 +3821,69 @@
       <c r="E4">
         <v>28.65</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>0.83</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>0.15</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <v>0.01</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="20">
         <v>1.9999999999999999E-6</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="36"/>
+      <c r="P4" t="s">
         <v>101</v>
       </c>
-      <c r="P4" s="20">
+      <c r="Q4" s="19">
         <f>101325/((8.31446261815324/E4*1000)*D4)/1000</f>
         <v>1.1795472504570127E-3</v>
       </c>
-      <c r="Q4">
-        <f>P4*G4</f>
+      <c r="R4">
+        <f>Q4*G4</f>
         <v>1.7693208756855192E-4</v>
       </c>
-      <c r="R4">
-        <f>P4*K4</f>
+      <c r="S4">
+        <f>Q4*K4</f>
         <v>0</v>
       </c>
-      <c r="S4" s="19">
-        <f>P4*N4</f>
+      <c r="T4" s="18">
+        <f>Q4*N4</f>
         <v>2.3590945009140252E-9</v>
       </c>
-      <c r="T4" s="18">
-        <f>P4*J4</f>
+      <c r="U4" s="17">
+        <f>Q4*J4</f>
         <v>5.8977362522850639E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="W4" s="17">
+        <f>Q4*I4</f>
+        <v>5.8977362522850639E-6</v>
+      </c>
+      <c r="X4" s="17">
+        <f>H4*Q4</f>
+        <v>1.1795472504570128E-5</v>
+      </c>
+      <c r="Z4" s="17">
+        <f t="shared" ref="Z4:Z7" si="0">Q4*F4</f>
+        <v>9.7902421787932048E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5">
         <v>450000</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="22">
         <v>1</v>
       </c>
       <c r="D5">
@@ -3776,50 +3892,65 @@
       <c r="E5">
         <v>2.59</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <v>1E-3</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="21">
         <v>0.83</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="21">
         <v>0.15</v>
       </c>
-      <c r="M5" s="22">
+      <c r="M5" s="21">
         <v>0.02</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="P5" t="s">
         <v>100</v>
       </c>
-      <c r="P5" s="20">
+      <c r="Q5" s="19">
         <f>101325/((8.31446261815324/E5*1000)*D5)/1000</f>
         <v>2.1767782489988911E-4</v>
       </c>
-      <c r="Q5">
-        <f>P5*G5</f>
+      <c r="R5">
+        <f>Q5*G5</f>
         <v>0</v>
       </c>
-      <c r="R5">
-        <f>P5*K5</f>
+      <c r="S5">
+        <f>Q5*K5</f>
         <v>1.8067259466690797E-4</v>
       </c>
-      <c r="S5" s="19">
-        <f>P5*N5</f>
+      <c r="T5" s="18">
+        <f>Q5*N5</f>
         <v>0</v>
       </c>
-      <c r="T5" s="24">
-        <f>P5*J5</f>
+      <c r="U5" s="23">
+        <f>Q5*J5</f>
         <v>2.1767782489988912E-7</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="V5" s="23">
+        <f>Q5*O5</f>
+        <v>2.1767782489988912E-7</v>
+      </c>
+      <c r="Y5" s="17">
+        <f>Q5*M5</f>
+        <v>4.3535564979977821E-6</v>
+      </c>
+      <c r="Z5" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6">
         <v>72000</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="22">
         <v>0.15</v>
       </c>
       <c r="D6">
@@ -3828,51 +3959,60 @@
       <c r="E6">
         <v>27.89</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>0.97</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="21">
         <v>0.01</v>
       </c>
-      <c r="M6" s="22">
+      <c r="M6" s="21">
         <v>0.02</v>
       </c>
-      <c r="N6" s="37">
-        <f>S6/P6</f>
+      <c r="N6" s="35">
+        <f>T6/Q6</f>
         <v>8.8149147713507682E-7</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="36"/>
+      <c r="P6" t="s">
         <v>99</v>
       </c>
-      <c r="P6" s="20">
+      <c r="Q6" s="19">
         <f>101325/((8.31446261815324/E6*1000)*D6)/1000</f>
         <v>2.6762533298464613E-3</v>
       </c>
-      <c r="Q6">
-        <f>P6*G6</f>
+      <c r="R6">
+        <f>Q6*G6</f>
         <v>0</v>
       </c>
-      <c r="R6">
-        <f>P6*K6</f>
+      <c r="S6">
+        <f>Q6*K6</f>
         <v>0</v>
       </c>
-      <c r="S6" s="36">
-        <f>S$4</f>
+      <c r="T6" s="34">
+        <f>T$4</f>
         <v>2.3590945009140252E-9</v>
       </c>
-      <c r="T6" s="18">
-        <f>P6*J6</f>
+      <c r="U6" s="17">
+        <f>Q6*J6</f>
         <v>2.6762533298464612E-5</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Y6" s="17">
+        <f>Q6*M6</f>
+        <v>5.3525066596929225E-5</v>
+      </c>
+      <c r="Z6" s="17">
+        <f t="shared" si="0"/>
+        <v>2.5959657299510675E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7">
         <v>41000</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="22">
         <v>1</v>
       </c>
       <c r="D7">
@@ -3881,49 +4021,267 @@
       <c r="E7">
         <v>27.95</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>0.98499999999999999</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="21">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="M7" s="22">
+      <c r="M7" s="21">
         <v>0.01</v>
       </c>
-      <c r="N7" s="37">
-        <f>S7/P7</f>
+      <c r="N7" s="35">
+        <f>T7/Q7</f>
         <v>6.3026398491514756E-7</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="36"/>
+      <c r="P7" t="s">
         <v>99</v>
       </c>
-      <c r="P7" s="20">
+      <c r="Q7" s="19">
         <f>101325/((8.31446261815324/E7*1000)*D7)/1000</f>
         <v>3.7430260293734381E-3</v>
       </c>
-      <c r="Q7">
-        <f>P7*G7</f>
+      <c r="R7">
+        <f>Q7*G7</f>
         <v>0</v>
       </c>
-      <c r="R7">
-        <f>P7*K7</f>
+      <c r="S7">
+        <f>Q7*K7</f>
         <v>0</v>
       </c>
-      <c r="S7" s="36">
-        <f>S$4</f>
+      <c r="T7" s="34">
+        <f>T$4</f>
         <v>2.3590945009140252E-9</v>
       </c>
-      <c r="T7" s="18">
-        <f>P7*J7</f>
+      <c r="U7" s="17">
+        <f>Q7*J7</f>
         <v>1.871513014686719E-5</v>
       </c>
+      <c r="Y7" s="17">
+        <f>Q7*M7</f>
+        <v>3.7430260293734381E-5</v>
+      </c>
+      <c r="Z7" s="17">
+        <f t="shared" si="0"/>
+        <v>3.6868806389328363E-3</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:T7" xr:uid="{45ED4848-3527-4D4F-9AC2-ED3907677CA1}"/>
   <mergeCells count="2">
-    <mergeCell ref="F1:N1"/>
-    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="F1:O1"/>
+    <mergeCell ref="R1:Z1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81489E60-0C69-41DB-9ED5-2FBC52367CC2}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3">
+        <f>B2/100</f>
+        <v>0.4</v>
+      </c>
+      <c r="C3">
+        <f>C2/100</f>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5">
+        <f>B3/B4</f>
+        <v>0.02</v>
+      </c>
+      <c r="C5">
+        <f>C3/C4</f>
+        <v>0.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0.999</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7">
+        <f>B6*B5</f>
+        <v>1.9980000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <f>C6*C5</f>
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="21">
+        <f>1-B6</f>
+        <v>1.0000000000000009E-3</v>
+      </c>
+      <c r="C8" s="21">
+        <f>1-C6</f>
+        <v>1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9">
+        <f>B8*B5</f>
+        <v>2.0000000000000019E-5</v>
+      </c>
+      <c r="C9">
+        <f>C8*C5</f>
+        <v>1.000000000000001E-4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <v>2333</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13">
+        <v>1333</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14">
+        <v>3000000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15">
+        <f>ROUND(B12/1000*B$14,-6)-B$14</f>
+        <v>4000000</v>
+      </c>
+      <c r="D15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16">
+        <f>ROUND(B13/1000*B$14,-6)-B$14</f>
+        <v>1000000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Body description compatibility fixes
Regex replacements in body descriptions (Grannus, Sirona, Nodens) to correct references to homeworld name or orbital parameters depending on which mods are installed: GPP, GEP_Primary, GEP_Rescale
</commit_message>
<xml_diff>
--- a/GEP_SpaceDust.xlsx
+++ b/GEP_SpaceDust.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louis\Documents\GitHub\Grannus-Expansion-Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A12082-3BCD-4523-B368-114D0388E8C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895D210B-D258-4CAE-9C70-27510068B1A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="570" windowWidth="26550" windowHeight="19155" xr2:uid="{CCF496B2-B669-4137-9B43-48A069A2A925}"/>
   </bookViews>
@@ -488,7 +488,7 @@
     <numFmt numFmtId="166" formatCode="0.000000000"/>
     <numFmt numFmtId="167" formatCode="0.0000%"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="0.0000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -656,12 +656,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,7 +665,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,7 +1022,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,24 +1039,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
       <c r="S1" s="16"/>
     </row>
     <row r="2" spans="1:20" s="11" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">
@@ -1125,35 +1125,35 @@
       <c r="A3" s="5">
         <v>12</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
       <c r="H3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="8" t="s">
         <v>141</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40"/>
-      <c r="R3" s="40"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
       <c r="S3" s="1">
         <f t="shared" ref="S3:S23" si="0">COUNTIFS(E3:R3,"&lt;&gt;",E3:R3,"&lt;&gt;-",E3:R3,"&lt;&gt;--")</f>
         <v>3</v>
@@ -1172,24 +1172,24 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="40"/>
+      <c r="I4" s="38"/>
       <c r="J4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="K4" s="40"/>
-      <c r="L4" s="40"/>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="40"/>
-      <c r="P4" s="40"/>
-      <c r="Q4" s="40"/>
-      <c r="R4" s="40"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
       <c r="S4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1208,20 +1208,20 @@
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40"/>
-      <c r="O5" s="40"/>
-      <c r="P5" s="40"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="40"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
       <c r="S5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1240,28 +1240,28 @@
       <c r="D6" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="40"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="40"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
       <c r="N6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O6" s="40"/>
+      <c r="O6" s="38"/>
       <c r="P6" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q6" s="40"/>
-      <c r="R6" s="41"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="39"/>
       <c r="S6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1280,20 +1280,20 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="40"/>
-      <c r="P7" s="40"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="40"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
       <c r="S7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1312,29 +1312,29 @@
       <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="8" t="s">
         <v>141</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="40"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="40"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
       <c r="N8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="O8" s="41"/>
+      <c r="O8" s="39"/>
       <c r="P8" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q8" s="40"/>
+      <c r="Q8" s="38"/>
       <c r="R8" s="8" t="s">
         <v>141</v>
       </c>
@@ -1357,24 +1357,24 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="40"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I9" s="40"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="41"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="39"/>
       <c r="S9" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1393,20 +1393,20 @@
       <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
       <c r="S10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1425,20 +1425,20 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40"/>
-      <c r="O11" s="40"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="40"/>
-      <c r="R11" s="40"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
       <c r="S11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1457,20 +1457,20 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40"/>
-      <c r="O12" s="40"/>
-      <c r="P12" s="40"/>
-      <c r="Q12" s="40"/>
-      <c r="R12" s="40"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
       <c r="S12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1489,16 +1489,16 @@
       <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
       <c r="H13" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I13" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="J13" s="40"/>
+      <c r="I13" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="38"/>
       <c r="K13" s="8" t="s">
         <v>141</v>
       </c>
@@ -1508,13 +1508,13 @@
       <c r="M13" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="N13" s="41"/>
+      <c r="N13" s="39"/>
       <c r="O13" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="41"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="39"/>
       <c r="S13" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1533,24 +1533,24 @@
       <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
       <c r="H14" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="I14" s="40"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="8" t="s">
         <v>141</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="L14" s="41"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="40"/>
-      <c r="P14" s="40"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
       <c r="Q14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1575,20 +1575,20 @@
       <c r="D15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="40"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
       <c r="S15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1607,28 +1607,28 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
       <c r="G16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="40"/>
+      <c r="H16" s="38"/>
       <c r="I16" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
       <c r="O16" s="8" t="s">
         <v>141</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="40"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="38"/>
       <c r="S16" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1647,20 +1647,20 @@
       <c r="D17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="41"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="39"/>
       <c r="S17" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1679,20 +1679,20 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="40"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
       <c r="S18" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1711,28 +1711,28 @@
       <c r="D19" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="40"/>
+      <c r="H19" s="38"/>
       <c r="I19" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
       <c r="O19" s="8" t="s">
         <v>141</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="40"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
       <c r="S19" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1751,20 +1751,20 @@
       <c r="D20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="40"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="41"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="39"/>
       <c r="S20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1783,20 +1783,20 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="40"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
       <c r="S21" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1815,20 +1815,20 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-      <c r="P22" s="40"/>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
       <c r="S22" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1847,20 +1847,20 @@
       <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="41"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="39"/>
       <c r="S23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1931,7 +1931,7 @@
         <f>IF(SUM(S3:S23)=SUM(E24:R24),SUM(S3:S23),"Err")</f>
         <v>35</v>
       </c>
-      <c r="T24" s="43" t="str">
+      <c r="T24" s="41" t="str">
         <f>"Ignored: "&amp;COUNTIF(E3:R23,"-")+COUNTIF(E3:R23,"--")</f>
         <v>Ignored: 1</v>
       </c>
@@ -1941,6 +1941,7 @@
     <filterColumn colId="18">
       <filters>
         <filter val="2"/>
+        <filter val="3"/>
         <filter val="35"/>
         <filter val="4"/>
         <filter val="5"/>
@@ -3532,33 +3533,33 @@
       <c r="E1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
       <c r="Q1" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
     </row>
     <row r="2" spans="1:27" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -3678,7 +3679,7 @@
         <v>99</v>
       </c>
       <c r="Q3" s="19">
-        <f>101325/((8.31446261815324/E3*1000)*D3)/1000</f>
+        <f t="shared" ref="Q3:Q8" si="0">101325/((8.31446261815324/E3*1000)*D3)/1000</f>
         <v>1.8858757889854774E-3</v>
       </c>
       <c r="R3">
@@ -3686,7 +3687,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <f>Q3*K3</f>
+        <f t="shared" ref="S3:S8" si="1">Q3*K3</f>
         <v>0</v>
       </c>
       <c r="T3" s="34">
@@ -3745,7 +3746,7 @@
         <v>101</v>
       </c>
       <c r="Q4" s="19">
-        <f>101325/((8.31446261815324/E4*1000)*D4)/1000</f>
+        <f t="shared" si="0"/>
         <v>1.1795472504570127E-3</v>
       </c>
       <c r="R4">
@@ -3753,7 +3754,7 @@
         <v>1.7693208756855192E-4</v>
       </c>
       <c r="S4">
-        <f>Q4*K4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T4" s="18">
@@ -3773,7 +3774,7 @@
         <v>1.1795472504570128E-5</v>
       </c>
       <c r="Z4" s="17">
-        <f t="shared" ref="Z4:Z7" si="0">Q4*F4</f>
+        <f t="shared" ref="Z4:Z7" si="2">Q4*F4</f>
         <v>9.7902421787932048E-4</v>
       </c>
     </row>
@@ -3812,7 +3813,7 @@
         <v>100</v>
       </c>
       <c r="Q5" s="19">
-        <f>101325/((8.31446261815324/E5*1000)*D5)/1000</f>
+        <f t="shared" si="0"/>
         <v>2.1767782489988911E-4</v>
       </c>
       <c r="R5">
@@ -3820,14 +3821,14 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <f>Q5*K5</f>
+        <f t="shared" si="1"/>
         <v>1.8067259466690797E-4</v>
       </c>
       <c r="T5" s="18">
         <f>Q5*N5</f>
         <v>0</v>
       </c>
-      <c r="U5" s="44">
+      <c r="U5" s="42">
         <f>Q5*J5</f>
         <v>0</v>
       </c>
@@ -3840,7 +3841,7 @@
         <v>4.3535564979977821E-6</v>
       </c>
       <c r="Z5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AA5" s="17">
@@ -3882,7 +3883,7 @@
         <v>99</v>
       </c>
       <c r="Q6" s="19">
-        <f>101325/((8.31446261815324/E6*1000)*D6)/1000</f>
+        <f t="shared" si="0"/>
         <v>2.6762533298464613E-3</v>
       </c>
       <c r="R6">
@@ -3890,7 +3891,7 @@
         <v>0</v>
       </c>
       <c r="S6">
-        <f>Q6*K6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T6" s="34">
@@ -3906,7 +3907,7 @@
         <v>5.3525066596929225E-5</v>
       </c>
       <c r="Z6" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.5959657299510675E-3</v>
       </c>
     </row>
@@ -3944,7 +3945,7 @@
         <v>99</v>
       </c>
       <c r="Q7" s="19">
-        <f>101325/((8.31446261815324/E7*1000)*D7)/1000</f>
+        <f t="shared" si="0"/>
         <v>3.7430260293734381E-3</v>
       </c>
       <c r="R7">
@@ -3952,7 +3953,7 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <f>Q7*K7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T7" s="34">
@@ -3968,7 +3969,7 @@
         <v>3.7430260293734381E-5</v>
       </c>
       <c r="Z7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.6868806389328363E-3</v>
       </c>
     </row>
@@ -3999,11 +4000,11 @@
         <v>99</v>
       </c>
       <c r="Q8" s="19">
-        <f>101325/((8.31446261815324/E8*1000)*D8)/1000</f>
+        <f t="shared" si="0"/>
         <v>3.6843198342129028E-6</v>
       </c>
       <c r="S8" s="19">
-        <f>Q8*K8</f>
+        <f t="shared" si="1"/>
         <v>3.3158878507916125E-6</v>
       </c>
       <c r="AA8" s="19">
@@ -4015,7 +4016,7 @@
       <c r="P10" t="s">
         <v>143</v>
       </c>
-      <c r="Q10" s="45">
+      <c r="Q10" s="43">
         <f>S5*26/1000000</f>
         <v>4.6974874613396069E-9</v>
       </c>
@@ -4024,7 +4025,7 @@
       <c r="P11" t="s">
         <v>144</v>
       </c>
-      <c r="Q11" s="45">
+      <c r="Q11" s="43">
         <f>Q10*0.75</f>
         <v>3.5231155960047052E-9</v>
       </c>
@@ -4033,7 +4034,7 @@
       <c r="P12" t="s">
         <v>145</v>
       </c>
-      <c r="Q12" s="45">
+      <c r="Q12" s="43">
         <f>Q10*1.25</f>
         <v>5.8718593266745087E-9</v>
       </c>
@@ -4283,24 +4284,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
       <c r="S1" s="16"/>
     </row>
     <row r="2" spans="1:20" s="11" customFormat="1" ht="73.5" x14ac:dyDescent="0.25">

</xml_diff>